<commit_message>
I change sparse model then change testing
</commit_message>
<xml_diff>
--- a/hybrid_searchTesting/timings_20_question_DBSF.xlsx
+++ b/hybrid_searchTesting/timings_20_question_DBSF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\hybrid_searchTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0831F2A-3047-45B5-B99E-1400B3AF42C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7816E0E2-DB71-4418-893D-3DB8CC9C1C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,19 +538,19 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>2.3090000000000002</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="C2">
-        <v>1.887</v>
+        <v>2.3769999999999998</v>
       </c>
       <c r="D2">
-        <v>0.78400000000000003</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="E2">
-        <v>1.8360000000000001</v>
+        <v>1.776</v>
       </c>
       <c r="F2">
-        <v>6.8159999999999998</v>
+        <v>5.4420000000000002</v>
       </c>
       <c r="G2">
         <v>0.81599999999999995</v>
@@ -564,19 +564,19 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.54400000000000004</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="C3">
-        <v>0.54500000000000004</v>
+        <v>2.2970000000000002</v>
       </c>
       <c r="D3">
-        <v>0.55000000000000004</v>
+        <v>0.62</v>
       </c>
       <c r="E3">
-        <v>1.357</v>
+        <v>1.1870000000000001</v>
       </c>
       <c r="F3">
-        <v>2.996</v>
+        <v>4.6459999999999999</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -590,22 +590,22 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.374</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="C4">
-        <v>0.42199999999999999</v>
+        <v>2.278</v>
       </c>
       <c r="D4">
-        <v>0.624</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="E4">
-        <v>1.575</v>
+        <v>1.5029999999999999</v>
       </c>
       <c r="F4">
-        <v>2.9950000000000001</v>
+        <v>4.9260000000000002</v>
       </c>
       <c r="G4">
-        <v>0.97399999999999998</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>28</v>
@@ -616,25 +616,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.34</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="C5">
-        <v>0.48199999999999998</v>
+        <v>2.3109999999999999</v>
       </c>
       <c r="D5">
-        <v>0.58599999999999997</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="E5">
-        <v>1.3919999999999999</v>
+        <v>1.3240000000000001</v>
       </c>
       <c r="F5">
-        <v>2.8010000000000002</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="G5">
         <v>0.81899999999999995</v>
       </c>
       <c r="H5">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -642,19 +642,19 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.35199999999999998</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="C6">
-        <v>0.625</v>
+        <v>3.1230000000000002</v>
       </c>
       <c r="D6">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="E6">
-        <v>1.605</v>
+        <v>1.5109999999999999</v>
       </c>
       <c r="F6">
-        <v>3.1309999999999998</v>
+        <v>5.96</v>
       </c>
       <c r="G6">
         <v>0.75600000000000001</v>
@@ -668,19 +668,19 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.42499999999999999</v>
+        <v>0.34</v>
       </c>
       <c r="C7">
-        <v>0.66</v>
+        <v>2.4049999999999998</v>
       </c>
       <c r="D7">
-        <v>0.621</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="E7">
-        <v>1.4870000000000001</v>
+        <v>1.5589999999999999</v>
       </c>
       <c r="F7">
-        <v>3.194</v>
+        <v>4.9020000000000001</v>
       </c>
       <c r="G7">
         <v>0.80900000000000005</v>
@@ -694,25 +694,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.47299999999999998</v>
+        <v>0.31</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>2.6269999999999998</v>
       </c>
       <c r="D8">
-        <v>0.54400000000000004</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="E8">
-        <v>1.3140000000000001</v>
+        <v>1.4139999999999999</v>
       </c>
       <c r="F8">
-        <v>2.831</v>
+        <v>4.9160000000000004</v>
       </c>
       <c r="G8">
         <v>0.78200000000000003</v>
       </c>
       <c r="H8">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -720,19 +720,19 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.33100000000000002</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="C9">
-        <v>0.58299999999999996</v>
+        <v>2.3210000000000002</v>
       </c>
       <c r="D9">
-        <v>0.63</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="E9">
-        <v>1.464</v>
+        <v>1.2270000000000001</v>
       </c>
       <c r="F9">
-        <v>3.008</v>
+        <v>4.468</v>
       </c>
       <c r="G9">
         <v>0.79900000000000004</v>
@@ -746,22 +746,22 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.34899999999999998</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="C10">
-        <v>0.49099999999999999</v>
+        <v>2.2690000000000001</v>
       </c>
       <c r="D10">
-        <v>0.55500000000000005</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="E10">
-        <v>1.5980000000000001</v>
+        <v>1.49</v>
       </c>
       <c r="F10">
-        <v>2.9940000000000002</v>
+        <v>4.8079999999999998</v>
       </c>
       <c r="G10">
-        <v>0.93</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="H10">
         <v>32</v>
@@ -772,25 +772,25 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.63900000000000001</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="C11">
-        <v>0.92300000000000004</v>
+        <v>2.2130000000000001</v>
       </c>
       <c r="D11">
-        <v>0.59499999999999997</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E11">
-        <v>1.4810000000000001</v>
+        <v>1.4530000000000001</v>
       </c>
       <c r="F11">
-        <v>3.6379999999999999</v>
+        <v>4.6340000000000003</v>
       </c>
       <c r="G11">
-        <v>0.79300000000000004</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="H11">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -798,22 +798,22 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0.55600000000000005</v>
+        <v>0.374</v>
       </c>
       <c r="C12">
-        <v>0.60399999999999998</v>
+        <v>2.3860000000000001</v>
       </c>
       <c r="D12">
-        <v>0.56100000000000005</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="E12">
-        <v>1.627</v>
+        <v>1.8939999999999999</v>
       </c>
       <c r="F12">
-        <v>3.3460000000000001</v>
+        <v>5.2510000000000003</v>
       </c>
       <c r="G12">
-        <v>0.91800000000000004</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="H12">
         <v>31</v>
@@ -824,22 +824,22 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0.36599999999999999</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="C13">
-        <v>0.46300000000000002</v>
+        <v>2.5329999999999999</v>
       </c>
       <c r="D13">
-        <v>0.63600000000000001</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="E13">
-        <v>2.1560000000000001</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="F13">
-        <v>3.6219999999999999</v>
+        <v>5.4450000000000003</v>
       </c>
       <c r="G13">
-        <v>0.90600000000000003</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="H13">
         <v>36</v>
@@ -850,22 +850,22 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>0.34899999999999998</v>
+        <v>0.316</v>
       </c>
       <c r="C14">
-        <v>0.52200000000000002</v>
+        <v>2.3959999999999999</v>
       </c>
       <c r="D14">
-        <v>0.59699999999999998</v>
+        <v>0.621</v>
       </c>
       <c r="E14">
-        <v>1.522</v>
+        <v>1.746</v>
       </c>
       <c r="F14">
-        <v>2.99</v>
+        <v>5.0780000000000003</v>
       </c>
       <c r="G14">
-        <v>0.71399999999999997</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="H14">
         <v>31</v>
@@ -876,25 +876,25 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>0.42299999999999999</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="C15">
-        <v>0.58699999999999997</v>
+        <v>2.4020000000000001</v>
       </c>
       <c r="D15">
-        <v>0.63600000000000001</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="E15">
-        <v>1.379</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="F15">
-        <v>3.024</v>
+        <v>4.9720000000000004</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -902,19 +902,19 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>0.314</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="C16">
-        <v>0.48399999999999999</v>
+        <v>2.3660000000000001</v>
       </c>
       <c r="D16">
-        <v>0.56999999999999995</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="E16">
-        <v>1.46</v>
+        <v>4.851</v>
       </c>
       <c r="F16">
-        <v>2.8340000000000001</v>
+        <v>8.1839999999999993</v>
       </c>
       <c r="G16">
         <v>0.872</v>
@@ -928,22 +928,22 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>0.32200000000000001</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="C17">
-        <v>0.50900000000000001</v>
+        <v>2.6360000000000001</v>
       </c>
       <c r="D17">
-        <v>0.60599999999999998</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="E17">
-        <v>2.274</v>
+        <v>2.5529999999999999</v>
       </c>
       <c r="F17">
-        <v>3.7130000000000001</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="H17">
         <v>31</v>
@@ -954,25 +954,25 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>0.65100000000000002</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="C18">
-        <v>0.56699999999999995</v>
+        <v>2.3109999999999999</v>
       </c>
       <c r="D18">
-        <v>0.64300000000000002</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="E18">
-        <v>1.627</v>
+        <v>1.306</v>
       </c>
       <c r="F18">
-        <v>3.4889999999999999</v>
+        <v>4.5339999999999998</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -980,25 +980,25 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>1.2969999999999999</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="C19">
-        <v>0.873</v>
+        <v>2.407</v>
       </c>
       <c r="D19">
-        <v>0.57099999999999995</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="E19">
-        <v>1.5629999999999999</v>
+        <v>1.5089999999999999</v>
       </c>
       <c r="F19">
-        <v>4.3040000000000003</v>
+        <v>4.8239999999999998</v>
       </c>
       <c r="G19">
         <v>0.90400000000000003</v>
       </c>
       <c r="H19">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1006,19 +1006,19 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0.36099999999999999</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="C20">
-        <v>0.57799999999999996</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D20">
-        <v>0.58599999999999997</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="E20">
-        <v>1.2949999999999999</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="F20">
-        <v>2.82</v>
+        <v>4.835</v>
       </c>
       <c r="G20">
         <v>0.88100000000000001</v>
@@ -1032,25 +1032,25 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>0.376</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="C21">
-        <v>0.63600000000000001</v>
+        <v>2.2650000000000001</v>
       </c>
       <c r="D21">
-        <v>0.628</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="E21">
-        <v>2.129</v>
+        <v>1.9650000000000001</v>
       </c>
       <c r="F21">
-        <v>3.77</v>
+        <v>5.1420000000000003</v>
       </c>
       <c r="G21">
         <v>0.89200000000000002</v>
       </c>
       <c r="H21">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1059,76 +1059,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04E9077-A5DD-4056-AB28-EACAB93A8DA2}">
-  <dimension ref="B5:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AA4059-20BF-4621-B8DD-FC40413F03ED}">
+  <dimension ref="B5:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="H5">
+      <c r="G5">
         <f>ROUND(AVERAGE(Sheet1!B2:B21),2)</f>
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="H7">
+      <c r="G7">
         <f>ROUND(AVERAGE(Sheet1!C2:C21),2)</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="H9">
+      <c r="G9">
         <f>ROUND(AVERAGE(Sheet1!D2:D21),2)</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="H11">
+      <c r="G11">
         <f>ROUND(AVERAGE(Sheet1!E2:E21),2)</f>
-        <v>1.61</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="H13">
+      <c r="G13">
         <f>ROUND(AVERAGE(Sheet1!F2:F21),2)</f>
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="H15">
+      <c r="G15">
         <f>ROUND(AVERAGE(Sheet1!G2:G21),2)</f>
         <v>0.87</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="H17">
-        <f>AVERAGE(Sheet1!H2:H21)</f>
-        <v>31.5</v>
+      <c r="G17">
+        <f>ROUND(AVERAGE(Sheet1!H2:H21),2)</f>
+        <v>31.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>